<commit_message>
poc changes excel doc
</commit_message>
<xml_diff>
--- a/data/2021draft.xlsx
+++ b/data/2021draft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdash/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c53fd0cc01813f56/Documents/Code/maxDemo/TRUFFLE/TRUFFLEdash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA31C983-A45D-5B41-A1CF-D927B21A5F7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{DA31C983-A45D-5B41-A1CF-D927B21A5F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6371EDC-CD5D-4E13-8AE6-C508587E3247}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="500" windowWidth="21920" windowHeight="16300" xr2:uid="{D12AAE90-AABA-3449-ACC7-08E3FE45A098}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15435" xr2:uid="{D12AAE90-AABA-3449-ACC7-08E3FE45A098}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,18 +507,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9392A3-5E21-7342-971C-8374374A01CF}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.625" customWidth="1"/>
+    <col min="4" max="4" width="28.125" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -552,7 +552,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -569,7 +569,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -586,7 +586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -603,7 +603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -620,7 +620,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -637,7 +637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -654,7 +654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -671,7 +671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -688,7 +688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -705,7 +705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -722,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -756,7 +756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -773,7 +773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -790,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -807,7 +807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -824,7 +824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -841,7 +841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -858,7 +858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -875,7 +875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -892,7 +892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -909,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -926,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -943,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -960,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -977,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -994,7 +994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>

</xml_diff>